<commit_message>
Added download file and fixed delete bug for sales form
</commit_message>
<xml_diff>
--- a/sales-reports/2023-12-13.xlsx
+++ b/sales-reports/2023-12-13.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Submission Date</t>
   </si>
@@ -58,54 +58,6 @@
   </si>
   <si>
     <t>File Upload</t>
-  </si>
-  <si>
-    <t>2023-12-13 12:05 p.m.</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2023-12-12 11:04 p.m.</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>CV</t>
-  </si>
-  <si>
-    <t>Crestama</t>
-  </si>
-  <si>
-    <t>Surabaya</t>
-  </si>
-  <si>
-    <t>Budi</t>
-  </si>
-  <si>
-    <t>1231231233</t>
-  </si>
-  <si>
-    <t>test email</t>
-  </si>
-  <si>
-    <t>Test Activity</t>
-  </si>
-  <si>
-    <t>1: Bagus</t>
-  </si>
-  <si>
-    <t>Joe mama</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>2023-12-12 11:06 p.m.</t>
-  </si>
-  <si>
-    <t>PT</t>
   </si>
 </sst>
 </file>
@@ -236,100 +188,6 @@
       </c>
       <c r="P1" s="1"/>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O3" t="s">
-        <v>28</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="0" useFirstPageNumber="false" blackAndWhite="false" orientation="portrait"/>

</xml_diff>